<commit_message>
updating name of articles
Carruthers et a.l 202 to Carruthers et al., 2021
</commit_message>
<xml_diff>
--- a/5_2_Metaanalysis_Meta/3_RelevantBiomarkers.xlsx
+++ b/5_2_Metaanalysis_Meta/3_RelevantBiomarkers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\_General\DoctoradoIndustrial2022\Publicaciones\METAANALISIS\Data\4_FullTestReading\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\GitHub\metaanalysisT2D\5_2_Metaanalysis_Meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F26820-2774-4D6E-A11D-EBCA76BD7FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138A4D55-FAA4-4C9A-8F84-0B144479A019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18060" yWindow="1200" windowWidth="10200" windowHeight="18540" xr2:uid="{1DDBD5C2-342B-48C5-8202-A2FA3020CE89}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{1DDBD5C2-342B-48C5-8202-A2FA3020CE89}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="237">
   <si>
     <t>ID</t>
   </si>
@@ -694,13 +694,55 @@
   </si>
   <si>
     <t>511_252</t>
+  </si>
+  <si>
+    <t>Sachdeva et al., 2024</t>
+  </si>
+  <si>
+    <t>Zou et al., 2020</t>
+  </si>
+  <si>
+    <t>Amorim et al., 2022</t>
+  </si>
+  <si>
+    <t>Li et al., 2023</t>
+  </si>
+  <si>
+    <t>Yan et al., 2024</t>
+  </si>
+  <si>
+    <t>Lewandowicz et al., 2015</t>
+  </si>
+  <si>
+    <t>Nimer et al., 2023</t>
+  </si>
+  <si>
+    <t>Abdulwahab et al., 2019</t>
+  </si>
+  <si>
+    <t>Kaur et al., 2012</t>
+  </si>
+  <si>
+    <t>Chen et al., 2020</t>
+  </si>
+  <si>
+    <t>Zhao et al., 2021</t>
+  </si>
+  <si>
+    <t>Yu et al., 2022</t>
+  </si>
+  <si>
+    <t>Zhao et al., 2024</t>
+  </si>
+  <si>
+    <t>An et al., 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -718,6 +760,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -740,15 +789,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{251FF37E-BA07-4D5F-AFB5-DB252FF05F9A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1062,21 +1114,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0AB9C7-24E7-4135-A23E-784D79C345C1}">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="5" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.3828125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.84375" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1089,10 +1142,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>179</v>
       </c>
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -1101,10 +1157,13 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>179</v>
       </c>
+      <c r="B3" t="s">
+        <v>223</v>
+      </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -1112,10 +1171,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>179</v>
       </c>
+      <c r="B4" t="s">
+        <v>223</v>
+      </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
@@ -1123,10 +1185,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>179</v>
       </c>
+      <c r="B5" t="s">
+        <v>223</v>
+      </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -1134,10 +1199,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>179</v>
       </c>
+      <c r="B6" t="s">
+        <v>223</v>
+      </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -1145,10 +1213,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>180</v>
       </c>
+      <c r="B7" t="s">
+        <v>224</v>
+      </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -1156,10 +1227,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>180</v>
       </c>
+      <c r="B8" t="s">
+        <v>224</v>
+      </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
@@ -1167,10 +1241,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>180</v>
       </c>
+      <c r="B9" t="s">
+        <v>224</v>
+      </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
@@ -1178,10 +1255,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>181</v>
       </c>
+      <c r="B10" t="s">
+        <v>225</v>
+      </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
@@ -1189,10 +1269,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>182</v>
       </c>
+      <c r="B11" t="s">
+        <v>226</v>
+      </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
@@ -1200,10 +1283,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>182</v>
       </c>
+      <c r="B12" t="s">
+        <v>226</v>
+      </c>
       <c r="C12" t="s">
         <v>24</v>
       </c>
@@ -1211,10 +1297,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>182</v>
       </c>
+      <c r="B13" t="s">
+        <v>226</v>
+      </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -1222,10 +1311,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>182</v>
       </c>
+      <c r="B14" t="s">
+        <v>226</v>
+      </c>
       <c r="C14" t="s">
         <v>29</v>
       </c>
@@ -1233,10 +1325,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>182</v>
       </c>
+      <c r="B15" t="s">
+        <v>226</v>
+      </c>
       <c r="C15" t="s">
         <v>31</v>
       </c>
@@ -1244,10 +1339,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>182</v>
       </c>
+      <c r="B16" t="s">
+        <v>226</v>
+      </c>
       <c r="C16" t="s">
         <v>32</v>
       </c>
@@ -1255,10 +1353,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>182</v>
       </c>
+      <c r="B17" t="s">
+        <v>226</v>
+      </c>
       <c r="C17" t="s">
         <v>35</v>
       </c>
@@ -1266,10 +1367,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>182</v>
       </c>
+      <c r="B18" t="s">
+        <v>226</v>
+      </c>
       <c r="C18" t="s">
         <v>37</v>
       </c>
@@ -1277,10 +1381,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>182</v>
       </c>
+      <c r="B19" t="s">
+        <v>226</v>
+      </c>
       <c r="C19" t="s">
         <v>39</v>
       </c>
@@ -1288,10 +1395,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>182</v>
       </c>
+      <c r="B20" t="s">
+        <v>226</v>
+      </c>
       <c r="C20" t="s">
         <v>41</v>
       </c>
@@ -1299,10 +1409,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>182</v>
       </c>
+      <c r="B21" t="s">
+        <v>226</v>
+      </c>
       <c r="C21" t="s">
         <v>43</v>
       </c>
@@ -1310,10 +1423,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>182</v>
       </c>
+      <c r="B22" t="s">
+        <v>226</v>
+      </c>
       <c r="C22" t="s">
         <v>45</v>
       </c>
@@ -1321,10 +1437,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>182</v>
       </c>
+      <c r="B23" t="s">
+        <v>226</v>
+      </c>
       <c r="C23" t="s">
         <v>47</v>
       </c>
@@ -1332,10 +1451,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>182</v>
       </c>
+      <c r="B24" t="s">
+        <v>226</v>
+      </c>
       <c r="C24" t="s">
         <v>49</v>
       </c>
@@ -1343,10 +1465,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>182</v>
       </c>
+      <c r="B25" t="s">
+        <v>226</v>
+      </c>
       <c r="C25" t="s">
         <v>51</v>
       </c>
@@ -1354,10 +1479,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>182</v>
       </c>
+      <c r="B26" t="s">
+        <v>226</v>
+      </c>
       <c r="C26" t="s">
         <v>53</v>
       </c>
@@ -1365,10 +1493,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>182</v>
       </c>
+      <c r="B27" t="s">
+        <v>226</v>
+      </c>
       <c r="C27" t="s">
         <v>55</v>
       </c>
@@ -1376,10 +1507,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>182</v>
       </c>
+      <c r="B28" t="s">
+        <v>226</v>
+      </c>
       <c r="C28" t="s">
         <v>27</v>
       </c>
@@ -1387,10 +1521,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>182</v>
       </c>
+      <c r="B29" t="s">
+        <v>226</v>
+      </c>
       <c r="C29" t="s">
         <v>57</v>
       </c>
@@ -1398,10 +1535,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>183</v>
       </c>
+      <c r="B30" t="s">
+        <v>227</v>
+      </c>
       <c r="C30" t="s">
         <v>60</v>
       </c>
@@ -1409,10 +1549,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>183</v>
       </c>
+      <c r="B31" t="s">
+        <v>227</v>
+      </c>
       <c r="C31" t="s">
         <v>61</v>
       </c>
@@ -1420,10 +1563,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>183</v>
       </c>
+      <c r="B32" t="s">
+        <v>227</v>
+      </c>
       <c r="C32" t="s">
         <v>61</v>
       </c>
@@ -1431,10 +1577,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>184</v>
       </c>
+      <c r="B33" t="s">
+        <v>228</v>
+      </c>
       <c r="C33" t="s">
         <v>63</v>
       </c>
@@ -1442,10 +1591,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>184</v>
       </c>
+      <c r="B34" t="s">
+        <v>228</v>
+      </c>
       <c r="C34" t="s">
         <v>69</v>
       </c>
@@ -1453,10 +1605,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>184</v>
       </c>
+      <c r="B35" t="s">
+        <v>228</v>
+      </c>
       <c r="C35" t="s">
         <v>70</v>
       </c>
@@ -1464,10 +1619,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>184</v>
       </c>
+      <c r="B36" t="s">
+        <v>228</v>
+      </c>
       <c r="C36" t="s">
         <v>71</v>
       </c>
@@ -1475,10 +1633,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>184</v>
       </c>
+      <c r="B37" t="s">
+        <v>228</v>
+      </c>
       <c r="C37" t="s">
         <v>72</v>
       </c>
@@ -1486,10 +1647,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>185</v>
       </c>
+      <c r="B38" t="s">
+        <v>229</v>
+      </c>
       <c r="C38" t="s">
         <v>20</v>
       </c>
@@ -1500,10 +1664,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>185</v>
       </c>
+      <c r="B39" t="s">
+        <v>229</v>
+      </c>
       <c r="C39" t="s">
         <v>93</v>
       </c>
@@ -1514,10 +1681,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>185</v>
       </c>
+      <c r="B40" t="s">
+        <v>229</v>
+      </c>
       <c r="C40" t="s">
         <v>75</v>
       </c>
@@ -1528,10 +1698,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>185</v>
       </c>
+      <c r="B41" t="s">
+        <v>229</v>
+      </c>
       <c r="C41" t="s">
         <v>78</v>
       </c>
@@ -1542,10 +1715,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>185</v>
       </c>
+      <c r="B42" t="s">
+        <v>229</v>
+      </c>
       <c r="C42" t="s">
         <v>81</v>
       </c>
@@ -1556,10 +1732,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>185</v>
       </c>
+      <c r="B43" t="s">
+        <v>229</v>
+      </c>
       <c r="C43" t="s">
         <v>101</v>
       </c>
@@ -1570,10 +1749,13 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>185</v>
       </c>
+      <c r="B44" t="s">
+        <v>229</v>
+      </c>
       <c r="C44" t="s">
         <v>87</v>
       </c>
@@ -1584,10 +1766,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>185</v>
       </c>
+      <c r="B45" t="s">
+        <v>229</v>
+      </c>
       <c r="C45" t="s">
         <v>90</v>
       </c>
@@ -1598,10 +1783,13 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>185</v>
       </c>
+      <c r="B46" t="s">
+        <v>229</v>
+      </c>
       <c r="C46" t="s">
         <v>95</v>
       </c>
@@ -1612,10 +1800,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>185</v>
       </c>
+      <c r="B47" t="s">
+        <v>229</v>
+      </c>
       <c r="C47" t="s">
         <v>98</v>
       </c>
@@ -1626,10 +1817,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>185</v>
       </c>
+      <c r="B48" t="s">
+        <v>229</v>
+      </c>
       <c r="C48" t="s">
         <v>84</v>
       </c>
@@ -1640,10 +1834,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>185</v>
       </c>
+      <c r="B49" t="s">
+        <v>229</v>
+      </c>
       <c r="C49" t="s">
         <v>104</v>
       </c>
@@ -1654,10 +1851,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>185</v>
       </c>
+      <c r="B50" t="s">
+        <v>229</v>
+      </c>
       <c r="C50" t="s">
         <v>107</v>
       </c>
@@ -1668,10 +1868,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>186</v>
       </c>
+      <c r="B51" t="s">
+        <v>230</v>
+      </c>
       <c r="C51" t="s">
         <v>110</v>
       </c>
@@ -1679,10 +1882,13 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>186</v>
       </c>
+      <c r="B52" t="s">
+        <v>230</v>
+      </c>
       <c r="C52" t="s">
         <v>93</v>
       </c>
@@ -1690,10 +1896,13 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>186</v>
       </c>
+      <c r="B53" t="s">
+        <v>230</v>
+      </c>
       <c r="C53" t="s">
         <v>113</v>
       </c>
@@ -1701,10 +1910,13 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>186</v>
       </c>
+      <c r="B54" t="s">
+        <v>230</v>
+      </c>
       <c r="C54" t="s">
         <v>115</v>
       </c>
@@ -1712,10 +1924,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>186</v>
       </c>
+      <c r="B55" t="s">
+        <v>230</v>
+      </c>
       <c r="C55" t="s">
         <v>117</v>
       </c>
@@ -1723,10 +1938,13 @@
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>186</v>
       </c>
+      <c r="B56" t="s">
+        <v>230</v>
+      </c>
       <c r="C56" t="s">
         <v>119</v>
       </c>
@@ -1734,10 +1952,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>186</v>
       </c>
+      <c r="B57" t="s">
+        <v>230</v>
+      </c>
       <c r="C57" t="s">
         <v>121</v>
       </c>
@@ -1745,10 +1966,13 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>186</v>
       </c>
+      <c r="B58" t="s">
+        <v>230</v>
+      </c>
       <c r="C58" t="s">
         <v>123</v>
       </c>
@@ -1756,10 +1980,13 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>186</v>
       </c>
+      <c r="B59" t="s">
+        <v>230</v>
+      </c>
       <c r="C59" t="s">
         <v>125</v>
       </c>
@@ -1767,10 +1994,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>186</v>
       </c>
+      <c r="B60" t="s">
+        <v>230</v>
+      </c>
       <c r="C60" t="s">
         <v>127</v>
       </c>
@@ -1778,10 +2008,13 @@
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>186</v>
       </c>
+      <c r="B61" t="s">
+        <v>230</v>
+      </c>
       <c r="C61" t="s">
         <v>129</v>
       </c>
@@ -1789,10 +2022,13 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>186</v>
       </c>
+      <c r="B62" t="s">
+        <v>230</v>
+      </c>
       <c r="C62" t="s">
         <v>131</v>
       </c>
@@ -1800,10 +2036,13 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>186</v>
       </c>
+      <c r="B63" t="s">
+        <v>230</v>
+      </c>
       <c r="C63" t="s">
         <v>133</v>
       </c>
@@ -1811,10 +2050,13 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>186</v>
       </c>
+      <c r="B64" t="s">
+        <v>230</v>
+      </c>
       <c r="C64" t="s">
         <v>135</v>
       </c>
@@ -1822,10 +2064,13 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>186</v>
       </c>
+      <c r="B65" t="s">
+        <v>230</v>
+      </c>
       <c r="C65" t="s">
         <v>137</v>
       </c>
@@ -1833,10 +2078,13 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>186</v>
       </c>
+      <c r="B66" t="s">
+        <v>230</v>
+      </c>
       <c r="C66" t="s">
         <v>139</v>
       </c>
@@ -1844,10 +2092,13 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>186</v>
       </c>
+      <c r="B67" t="s">
+        <v>230</v>
+      </c>
       <c r="C67" t="s">
         <v>141</v>
       </c>
@@ -1855,10 +2106,13 @@
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>186</v>
       </c>
+      <c r="B68" t="s">
+        <v>230</v>
+      </c>
       <c r="C68" t="s">
         <v>143</v>
       </c>
@@ -1866,10 +2120,13 @@
         <v>144</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>186</v>
       </c>
+      <c r="B69" t="s">
+        <v>230</v>
+      </c>
       <c r="C69" t="s">
         <v>145</v>
       </c>
@@ -1877,10 +2134,13 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>186</v>
       </c>
+      <c r="B70" t="s">
+        <v>230</v>
+      </c>
       <c r="C70" t="s">
         <v>147</v>
       </c>
@@ -1888,10 +2148,13 @@
         <v>148</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>186</v>
       </c>
+      <c r="B71" t="s">
+        <v>230</v>
+      </c>
       <c r="C71" t="s">
         <v>149</v>
       </c>
@@ -1899,10 +2162,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>186</v>
       </c>
+      <c r="B72" t="s">
+        <v>230</v>
+      </c>
       <c r="C72" t="s">
         <v>151</v>
       </c>
@@ -1910,10 +2176,13 @@
         <v>152</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>186</v>
       </c>
+      <c r="B73" t="s">
+        <v>230</v>
+      </c>
       <c r="C73" t="s">
         <v>153</v>
       </c>
@@ -1921,10 +2190,13 @@
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>187</v>
       </c>
+      <c r="B74" t="s">
+        <v>231</v>
+      </c>
       <c r="C74" t="s">
         <v>155</v>
       </c>
@@ -1932,10 +2204,13 @@
         <v>156</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>187</v>
       </c>
+      <c r="B75" t="s">
+        <v>231</v>
+      </c>
       <c r="C75" t="s">
         <v>127</v>
       </c>
@@ -1943,10 +2218,13 @@
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>188</v>
       </c>
+      <c r="B76" t="s">
+        <v>232</v>
+      </c>
       <c r="C76" t="s">
         <v>87</v>
       </c>
@@ -1957,10 +2235,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>188</v>
       </c>
+      <c r="B77" t="s">
+        <v>232</v>
+      </c>
       <c r="C77" t="s">
         <v>159</v>
       </c>
@@ -1971,10 +2252,13 @@
         <v>160</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>188</v>
       </c>
+      <c r="B78" t="s">
+        <v>232</v>
+      </c>
       <c r="C78" t="s">
         <v>162</v>
       </c>
@@ -1985,10 +2269,13 @@
         <v>163</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>189</v>
       </c>
+      <c r="B79" t="s">
+        <v>233</v>
+      </c>
       <c r="C79" t="s">
         <v>165</v>
       </c>
@@ -1999,10 +2286,13 @@
         <v>166</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>189</v>
       </c>
+      <c r="B80" t="s">
+        <v>233</v>
+      </c>
       <c r="C80" t="s">
         <v>168</v>
       </c>
@@ -2013,10 +2303,13 @@
         <v>169</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>189</v>
       </c>
+      <c r="B81" t="s">
+        <v>233</v>
+      </c>
       <c r="C81" t="s">
         <v>170</v>
       </c>
@@ -2027,10 +2320,13 @@
         <v>171</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>189</v>
       </c>
+      <c r="B82" t="s">
+        <v>233</v>
+      </c>
       <c r="C82" t="s">
         <v>174</v>
       </c>
@@ -2041,10 +2337,13 @@
         <v>175</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>190</v>
       </c>
+      <c r="B83" t="s">
+        <v>234</v>
+      </c>
       <c r="C83" t="s">
         <v>176</v>
       </c>
@@ -2055,10 +2354,13 @@
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>191</v>
       </c>
+      <c r="B84" t="s">
+        <v>235</v>
+      </c>
       <c r="C84" t="s">
         <v>192</v>
       </c>
@@ -2069,10 +2371,13 @@
         <v>209</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>191</v>
       </c>
+      <c r="B85" t="s">
+        <v>235</v>
+      </c>
       <c r="C85" t="s">
         <v>199</v>
       </c>
@@ -2083,10 +2388,13 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>191</v>
       </c>
+      <c r="B86" t="s">
+        <v>235</v>
+      </c>
       <c r="C86" t="s">
         <v>200</v>
       </c>
@@ -2097,10 +2405,13 @@
         <v>207</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>191</v>
       </c>
+      <c r="B87" t="s">
+        <v>235</v>
+      </c>
       <c r="C87" t="s">
         <v>201</v>
       </c>
@@ -2111,10 +2422,13 @@
         <v>206</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>191</v>
       </c>
+      <c r="B88" t="s">
+        <v>235</v>
+      </c>
       <c r="C88" t="s">
         <v>202</v>
       </c>
@@ -2125,10 +2439,13 @@
         <v>205</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>191</v>
       </c>
+      <c r="B89" t="s">
+        <v>235</v>
+      </c>
       <c r="C89" t="s">
         <v>203</v>
       </c>
@@ -2139,10 +2456,13 @@
         <v>204</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>222</v>
       </c>
+      <c r="B90" t="s">
+        <v>236</v>
+      </c>
       <c r="C90" t="s">
         <v>210</v>
       </c>
@@ -2153,10 +2473,13 @@
         <v>212</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>222</v>
       </c>
+      <c r="B91" t="s">
+        <v>236</v>
+      </c>
       <c r="C91" t="s">
         <v>213</v>
       </c>
@@ -2167,10 +2490,13 @@
         <v>215</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>222</v>
       </c>
+      <c r="B92" t="s">
+        <v>236</v>
+      </c>
       <c r="C92" t="s">
         <v>217</v>
       </c>
@@ -2181,9 +2507,12 @@
         <v>216</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>222</v>
+      </c>
+      <c r="B93" t="s">
+        <v>236</v>
       </c>
       <c r="C93" t="s">
         <v>220</v>

</xml_diff>